<commit_message>
final version of dvp
</commit_message>
<xml_diff>
--- a/exported_session.xlsx
+++ b/exported_session.xlsx
@@ -115,22 +115,22 @@
     <t>RH</t>
   </si>
   <si>
-    <t>sub000</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>iDAPT000</t>
-  </si>
-  <si>
-    <t>unknown gender</t>
-  </si>
-  <si>
-    <t>unknown walkway</t>
-  </si>
-  <si>
-    <t>observer</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>wet</t>
+  </si>
+  <si>
+    <t>sub007</t>
+  </si>
+  <si>
+    <t>iDAPT343</t>
+  </si>
+  <si>
+    <t>Wu</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:AG3"/>
+      <selection activeCell="C3" sqref="C3:AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,186 +619,168 @@
     </row>
     <row r="2" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="W2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Y2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Z2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA2" t="s">
         <v>38</v>
       </c>
       <c r="AB2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC2" s="3">
-        <v>41255</v>
+        <v>43864</v>
       </c>
       <c r="AD2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
+        <v>0.62708333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="W3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Y3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Z3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA3" t="s">
         <v>38</v>
       </c>
       <c r="AB3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC3" s="3">
-        <v>41255</v>
+        <v>43864</v>
       </c>
       <c r="AD3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
+        <v>0.62708333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>